<commit_message>
Remove venv from tracking and add to .gitignore
</commit_message>
<xml_diff>
--- a/top_videos_scored.xlsx
+++ b/top_videos_scored.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,55 +475,60 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>duration_str</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>video_id</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>url</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>likes_per_view</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>comments_per_minute</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>views_per_day</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>norm_likes_per_view</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>norm_comments_per_minute</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>norm_views_per_day</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>norm_views</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>final_score</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
@@ -544,10 +549,10 @@
         <v>44169.72681712963</v>
       </c>
       <c r="D2" t="n">
-        <v>2937483</v>
+        <v>2940151</v>
       </c>
       <c r="E2" t="n">
-        <v>75902</v>
+        <v>75970</v>
       </c>
       <c r="F2" t="n">
         <v>2245</v>
@@ -557,39 +562,44 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>4:33:03</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>xfzGZB4HhEE</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>https://www.youtube.com/watch?v=xfzGZB4HhEE</t>
         </is>
       </c>
-      <c r="J2" t="n">
-        <v>0.02583912826048695</v>
-      </c>
       <c r="K2" t="n">
+        <v>0.02583880895913169</v>
+      </c>
+      <c r="L2" t="n">
         <v>8.218927329306242</v>
       </c>
-      <c r="L2" t="n">
-        <v>1816.625231910946</v>
-      </c>
       <c r="M2" t="n">
-        <v>0.1997626111873345</v>
+        <v>1814.908024691358</v>
       </c>
       <c r="N2" t="n">
-        <v>0.03045671954948187</v>
+        <v>0.350782384575447</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9999999999994332</v>
+        <v>0.03495405875667099</v>
       </c>
       <c r="P2" t="n">
+        <v>0.7974064119635269</v>
+      </c>
+      <c r="Q2" t="n">
         <v>0.9999999999999997</v>
       </c>
-      <c r="Q2" t="n">
-        <v>5.660201272659267</v>
-      </c>
       <c r="R2" t="n">
+        <v>5.514474507130263</v>
+      </c>
+      <c r="S2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -608,245 +618,196 @@
         <v>45225.52559027778</v>
       </c>
       <c r="D3" t="n">
-        <v>1002282</v>
+        <v>1003867</v>
       </c>
       <c r="E3" t="n">
-        <v>16850</v>
+        <v>16878</v>
       </c>
       <c r="F3" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G3" t="n">
         <v>179.33</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>2:59:20</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>9Y3yaoi9rUQ</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>https://www.youtube.com/watch?v=9Y3yaoi9rUQ</t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>0.01681163584699715</v>
-      </c>
       <c r="K3" t="n">
-        <v>2.078805105054896</v>
+        <v>0.01681298419013674</v>
       </c>
       <c r="L3" t="n">
-        <v>1786.598930481283</v>
+        <v>2.084378309089896</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0121733997944631</v>
+        <v>1779.906028368794</v>
       </c>
       <c r="N3" t="n">
-        <v>0.003581667953219282</v>
+        <v>0.2282496339275403</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9829807992111056</v>
+        <v>0.008864597406436569</v>
       </c>
       <c r="P3" t="n">
-        <v>0.3341777674254416</v>
+        <v>0.7816251143145888</v>
       </c>
       <c r="Q3" t="n">
-        <v>3.660981467774028</v>
+        <v>0.3414006720401305</v>
       </c>
       <c r="R3" t="n">
+        <v>3.730154783619521</v>
+      </c>
+      <c r="S3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>I Tried Day Trading w/ a Trading Bot Algorithm</t>
+          <t>He Makes a Living Algo Trading in Forex - Scott Welsh | Trader Interview</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Daniel Inskeep</t>
+          <t>Etienne Crete - Desire To TRADE</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44678.58370370371</v>
+        <v>44731.45846064815</v>
       </c>
       <c r="D4" t="n">
-        <v>1017770</v>
+        <v>48993</v>
       </c>
       <c r="E4" t="n">
-        <v>19911</v>
+        <v>1100</v>
       </c>
       <c r="F4" t="n">
-        <v>1340</v>
+        <v>68</v>
       </c>
       <c r="G4" t="n">
-        <v>14.02</v>
+        <v>34.47</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>lQlWlrdGaz0</t>
+          <t>34:28</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=lQlWlrdGaz0</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>0.01956335910863947</v>
+          <t>TKVE6DL7ubU</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=TKVE6DL7ubU</t>
+        </is>
       </c>
       <c r="K4" t="n">
-        <v>94.90084985835695</v>
+        <v>0.02245218704712918</v>
       </c>
       <c r="L4" t="n">
-        <v>918.5649819494585</v>
+        <v>1.967023430720278</v>
       </c>
       <c r="M4" t="n">
-        <v>0.06935357486185548</v>
+        <v>46.30718336483932</v>
       </c>
       <c r="N4" t="n">
-        <v>0.4098597762558189</v>
+        <v>0.3048062983004695</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4909706828218275</v>
+        <v>0.008365501946705834</v>
       </c>
       <c r="P4" t="n">
-        <v>0.3395065445075714</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.17970541457783</v>
+        <v>0.0166139286252429</v>
       </c>
       <c r="R4" t="n">
+        <v>0.9643777560453058</v>
+      </c>
+      <c r="S4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>How Do Stock Trading Algorithms Work?</t>
+          <t>7 Algo Trading Strategies (Backtest And Rules)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Concerning Reality</t>
+          <t>Quantified Strategies</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>43759.63541666666</v>
+        <v>45194.54184027778</v>
       </c>
       <c r="D5" t="n">
-        <v>127870</v>
+        <v>31246</v>
       </c>
       <c r="E5" t="n">
-        <v>2200</v>
+        <v>505</v>
       </c>
       <c r="F5" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="G5" t="n">
-        <v>7.02</v>
+        <v>9.42</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>OPm_EDTrz7Y</t>
+          <t>9:25</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OPm_EDTrz7Y</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>0.01720497380151717</v>
+          <t>NojfYk31_xI</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=NojfYk31_xI</t>
+        </is>
       </c>
       <c r="K5" t="n">
-        <v>8.286516853932586</v>
+        <v>0.01616206874479933</v>
       </c>
       <c r="L5" t="n">
-        <v>63.0833744449926</v>
+        <v>1.260504201680672</v>
       </c>
       <c r="M5" t="n">
-        <v>0.02034687181965543</v>
+        <v>52.51428571428571</v>
       </c>
       <c r="N5" t="n">
-        <v>0.03075255599953255</v>
+        <v>0.2194129389996283</v>
       </c>
       <c r="O5" t="n">
-        <v>0.006075355871689034</v>
+        <v>0.005360764995630636</v>
       </c>
       <c r="P5" t="n">
-        <v>0.03332894085394615</v>
+        <v>0.002798586938051013</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.2074296767809908</v>
+        <v>0.01057754022699976</v>
       </c>
       <c r="R5" t="n">
+        <v>0.6985111882582986</v>
+      </c>
+      <c r="S5" t="n">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>7 Algo Trading Strategies (Backtest And Rules)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Quantified Strategies</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>45194.54184027778</v>
-      </c>
-      <c r="D6" t="n">
-        <v>31000</v>
-      </c>
-      <c r="E6" t="n">
-        <v>503</v>
-      </c>
-      <c r="F6" t="n">
-        <v>12</v>
-      </c>
-      <c r="G6" t="n">
-        <v>9.42</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>NojfYk31_xI</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=NojfYk31_xI</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>0.0162258064516129</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1.260504201680672</v>
-      </c>
-      <c r="L6" t="n">
-        <v>52.36486486486486</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve video suggestion layout and fix UI issues
</commit_message>
<xml_diff>
--- a/top_videos_scored.xlsx
+++ b/top_videos_scored.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,67 +537,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Algorithmic Trading Using Python - Full Course</t>
+          <t>How The Economic Machine Works by Ray Dalio</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>freeCodeCamp.org</t>
+          <t>Principles by Ray Dalio</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44169.72681712963</v>
+        <v>41539.75540509259</v>
       </c>
       <c r="D2" t="n">
-        <v>2940151</v>
+        <v>43654314</v>
       </c>
       <c r="E2" t="n">
-        <v>75970</v>
+        <v>671653</v>
       </c>
       <c r="F2" t="n">
-        <v>2245</v>
+        <v>24368</v>
       </c>
       <c r="G2" t="n">
-        <v>273.05</v>
+        <v>31</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>4:33:03</t>
+          <t>31:00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>xfzGZB4HhEE</t>
+          <t>PHe0bXAIuk0</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=xfzGZB4HhEE</t>
+          <t>https://www.youtube.com/watch?v=PHe0bXAIuk0</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0.02583880895913169</v>
+        <v>0.01538571880891314</v>
       </c>
       <c r="L2" t="n">
-        <v>8.218927329306242</v>
+        <v>783.5369774919614</v>
       </c>
       <c r="M2" t="n">
-        <v>1814.908024691358</v>
+        <v>10271.60329411765</v>
       </c>
       <c r="N2" t="n">
-        <v>0.350782384575447</v>
+        <v>0.170419573613995</v>
       </c>
       <c r="O2" t="n">
-        <v>0.03495405875667099</v>
+        <v>0.4489254980311678</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7974064119635269</v>
+        <v>0.9999999999999019</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.9999999999999997</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>5.514474507130263</v>
+        <v>6.409109716904027</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
@@ -606,67 +606,67 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Algorithmic Trading – Machine Learning &amp; Quant Strategies Course with Python</t>
+          <t>Every Major Economic Theory Explained in 20 Minutes</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>freeCodeCamp.org</t>
+          <t>Adam's Axiom</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45225.52559027778</v>
+        <v>45649.54217592593</v>
       </c>
       <c r="D3" t="n">
-        <v>1003867</v>
+        <v>498390</v>
       </c>
       <c r="E3" t="n">
-        <v>16878</v>
+        <v>18280</v>
       </c>
       <c r="F3" t="n">
-        <v>374</v>
+        <v>507</v>
       </c>
       <c r="G3" t="n">
-        <v>179.33</v>
+        <v>20.62</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2:59:20</t>
+          <t>20:37</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>9Y3yaoi9rUQ</t>
+          <t>dQ_UPQa3CUE</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9Y3yaoi9rUQ</t>
+          <t>https://www.youtube.com/watch?v=dQ_UPQa3CUE</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0.01681298419013674</v>
+        <v>0.03667810349324826</v>
       </c>
       <c r="L3" t="n">
-        <v>2.084378309089896</v>
+        <v>24.46911196911197</v>
       </c>
       <c r="M3" t="n">
-        <v>1779.906028368794</v>
+        <v>3534.68085106383</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2282496339275403</v>
+        <v>0.5211902786773303</v>
       </c>
       <c r="O3" t="n">
-        <v>0.008864597406436569</v>
+        <v>0.01401951483167455</v>
       </c>
       <c r="P3" t="n">
-        <v>0.7816251143145888</v>
+        <v>0.3392962401352193</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.3414006720401305</v>
+        <v>0.01138080102074723</v>
       </c>
       <c r="R3" t="n">
-        <v>3.730154783619521</v>
+        <v>2.632260188142492</v>
       </c>
       <c r="S3" t="n">
         <v>2</v>
@@ -675,67 +675,67 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>He Makes a Living Algo Trading in Forex - Scott Welsh | Trader Interview</t>
+          <t>Intro to Economics: Crash Course Econ #1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Etienne Crete - Desire To TRADE</t>
+          <t>CrashCourse</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44731.45846064815</v>
+        <v>42193.94049768519</v>
       </c>
       <c r="D4" t="n">
-        <v>48993</v>
+        <v>8264493</v>
       </c>
       <c r="E4" t="n">
-        <v>1100</v>
+        <v>116672</v>
       </c>
       <c r="F4" t="n">
-        <v>68</v>
+        <v>4446</v>
       </c>
       <c r="G4" t="n">
-        <v>34.47</v>
+        <v>12.15</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>34:28</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>TKVE6DL7ubU</t>
+          <t>3ez10ADR_gM</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TKVE6DL7ubU</t>
+          <t>https://www.youtube.com/watch?v=3ez10ADR_gM</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0.02245218704712918</v>
+        <v>0.01411726042964765</v>
       </c>
       <c r="L4" t="n">
-        <v>1.967023430720278</v>
+        <v>362.9387755102041</v>
       </c>
       <c r="M4" t="n">
-        <v>46.30718336483932</v>
+        <v>2298.246106785317</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3048062983004695</v>
+        <v>0.1495229926703963</v>
       </c>
       <c r="O4" t="n">
-        <v>0.008365501946705834</v>
+        <v>0.2079448388923191</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>0.2180365564625309</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0166139286252429</v>
+        <v>0.1892872809526882</v>
       </c>
       <c r="R4" t="n">
-        <v>0.9643777560453058</v>
+        <v>1.897142887088796</v>
       </c>
       <c r="S4" t="n">
         <v>3</v>
@@ -744,70 +744,346 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7 Algo Trading Strategies (Backtest And Rules)</t>
+          <t>What Everyone Gets Wrong About Global Debt | Economics Explained</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Quantified Strategies</t>
+          <t>Economics Explained</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45194.54184027778</v>
+        <v>45109.56671296297</v>
       </c>
       <c r="D5" t="n">
-        <v>31246</v>
+        <v>1641344</v>
       </c>
       <c r="E5" t="n">
-        <v>505</v>
+        <v>29325</v>
       </c>
       <c r="F5" t="n">
-        <v>12</v>
+        <v>1392</v>
       </c>
       <c r="G5" t="n">
-        <v>9.42</v>
+        <v>16.68</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>9:25</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>NojfYk31_xI</t>
+          <t>IAqj30s4lH8</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NojfYk31_xI</t>
+          <t>https://www.youtube.com/watch?v=IAqj30s4lH8</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0.01616206874479933</v>
+        <v>0.01786645578257818</v>
       </c>
       <c r="L5" t="n">
-        <v>1.260504201680672</v>
+        <v>82.95589988081048</v>
       </c>
       <c r="M5" t="n">
-        <v>52.51428571428571</v>
+        <v>2410.196769456682</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2194129389996283</v>
+        <v>0.2112872298314481</v>
       </c>
       <c r="O5" t="n">
-        <v>0.005360764995630636</v>
+        <v>0.04752936968950978</v>
       </c>
       <c r="P5" t="n">
-        <v>0.002798586938051013</v>
+        <v>0.2290157868710058</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.01057754022699976</v>
+        <v>0.03756367843869182</v>
       </c>
       <c r="R5" t="n">
-        <v>0.6985111882582986</v>
+        <v>1.491095146363765</v>
       </c>
       <c r="S5" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>The Most Important Economic Schools of Thought | Economics Explained</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Economics Explained</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>44084.53758101852</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1841614</v>
+      </c>
+      <c r="E6" t="n">
+        <v>45281</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3174</v>
+      </c>
+      <c r="G6" t="n">
+        <v>26.08</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>26:05</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>o6UXRZ2XwgU</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=o6UXRZ2XwgU</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>0.02458767146644194</v>
+      </c>
+      <c r="L6" t="n">
+        <v>121.2375859434683</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1079.492379835873</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.3220125243094374</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.06946276335800169</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.09851088631401388</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.04215147887553508</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1.484798716337427</v>
+      </c>
+      <c r="S6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>How The Economy Works For DUMMIES: Global Economics 101 -Robert Kiyosaki</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>The Rich Dad Channel</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>43585.81953703704</v>
+      </c>
+      <c r="D7" t="n">
+        <v>165339</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3975</v>
+      </c>
+      <c r="F7" t="n">
+        <v>215</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>3:30</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>9iV55N2nuJY</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=9iV55N2nuJY</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>0.02404151470614918</v>
+      </c>
+      <c r="L7" t="n">
+        <v>59.72222222222222</v>
+      </c>
+      <c r="M7" t="n">
+        <v>75.01769509981851</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.3130151388721953</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.03421769377172024</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.003751243307205069</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1.014983290774436</v>
+      </c>
+      <c r="S7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Introduction to Economics Part 1 - Professor Ryan</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Prof Ryan</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>43613.19787037037</v>
+      </c>
+      <c r="D8" t="n">
+        <v>189733</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4337</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>qnEZQRpWWi8</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=qnEZQRpWWi8</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>0.02285843791011579</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>87.15342214056041</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.2935251339694559</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.001190175566408197</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.004310062920009556</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.8927660544476114</v>
+      </c>
+      <c r="S8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Thomas Sowell -- Basic Economics</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Hoover Institution</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>40549.97076388889</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2520647</v>
+      </c>
+      <c r="E9" t="n">
+        <v>44076</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1256</v>
+      </c>
+      <c r="G9" t="n">
+        <v>33.53</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>33:32</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>bOMksnSaAJ4</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=bOMksnSaAJ4</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>0.01748598673277139</v>
+      </c>
+      <c r="L9" t="n">
+        <v>37.34760630389533</v>
+      </c>
+      <c r="M9" t="n">
+        <v>481.0395038167939</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.2050193834237279</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.02139821507073698</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.03981938902724899</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.05770681863701207</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.8927263847684287</v>
+      </c>
+      <c r="S9" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>